<commit_message>
fixes, refactorings and enhancements for excel, added read example
</commit_message>
<xml_diff>
--- a/data/test/TestSheet1.xlsx
+++ b/data/test/TestSheet1.xlsx
@@ -69,6 +69,7 @@
   <fonts count="4">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -159,19 +160,19 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="B7" activeCellId="0" pane="topLeft" sqref="B7"/>
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -185,7 +186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
         <v>5</v>
       </c>
@@ -199,7 +200,7 @@
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
@@ -213,7 +214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
         <v>11</v>
       </c>

</xml_diff>